<commit_message>
correct incomplete sentence in excel file
</commit_message>
<xml_diff>
--- a/www/Titelblatt.xlsx
+++ b/www/Titelblatt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszfea\GitHub\Shiny-Apps\MPE-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszhas\Documents\repos\MPE-Tool\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7248" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>Diese Raumeinheit wurde aufgrund der Filterung nach Bauträgerschaft gebildet. Siehe entsprechender Abschnitt.</t>
   </si>
   <si>
-    <t>Der Median ist der Wert, der die Mietpreise in zwei gleich grosse Hälften teilt, d.h. die eine Hälfte der Mietpreise kleiner als der Median, die andere Hälfte grösser.</t>
-  </si>
-  <si>
     <t>Die geschätzten Preise sind mit 95-%-Konfidenzintervallen unterlegt. Diese bezeichnen den Bereich, der bei unendlicher Wiederholung eines Zufallsexperiments mit einer Wahrscheinlichkeit von 95 Prozent den wahren Wert der Grundgesamtheit einschliesst. In der MPE liegen die 95-%-Konfidenzintervalle gesamtstädtisch ungefähr bei 4 Prozent der ausgewiesenen Medianpreise und Mittelwerte (absolute Breite des Konfidenzintervalls geteilt durch Schätzwert). Bei kleineren Raumeinheiten (z.B. Quartiere) sind die Unsicherheiten höher; die Konfidenzintervalle der ausgewiesenen Werte liegen im Bereich von 4 bis 8 Prozent und können unter Umständen bis gegen 20 Prozent steigen.</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>Die Detaildaten der Mietpreiserhebung 2022 sind auf einem Abruftool verfügbar, das erreichbar ist unter: https://www.stadt-zuerich.ch/prd/de/index/statistik/publikationen-angebote/datenbanken-anwendungen/mietpreiserhebung.html</t>
+  </si>
+  <si>
+    <t>Der Median ist der Wert, der die Mietpreise in zwei gleich grosse Hälften teilt, d.h. die eine Hälfte der Mietpreise ist kleiner als der Median, die andere Hälfte grösser.</t>
   </si>
 </sst>
 </file>
@@ -487,12 +487,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -509,27 +509,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
@@ -537,12 +537,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -561,13 +561,13 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
@@ -579,7 +579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -587,7 +587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -595,7 +595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
@@ -603,7 +603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
@@ -611,23 +611,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -635,20 +635,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>